<commit_message>
update xlsx for specification
</commit_message>
<xml_diff>
--- a/src/test/resources/sample/SomeDomainTemplate.xlsx
+++ b/src/test/resources/sample/SomeDomainTemplate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Renommer</t>
   </si>
   <si>
     <t>Tags</t>
@@ -2245,7 +2248,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2255,8 +2258,8 @@
     <col min="2" max="2" width="26.3516" style="20" customWidth="1"/>
     <col min="3" max="3" width="4.17188" style="20" customWidth="1"/>
     <col min="4" max="4" width="24.8516" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.8516" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="20" customWidth="1"/>
+    <col min="5" max="6" width="10.8516" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="10.8516" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -2275,20 +2278,24 @@
       <c r="E1" t="s" s="21">
         <v>19</v>
       </c>
+      <c r="F1" t="s" s="21">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="21">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" t="s" s="21">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s" s="21">
         <v>23</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" t="s" s="21">
+        <v>24</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
@@ -2297,6 +2304,7 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="22"/>
@@ -2304,6 +2312,7 @@
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="22"/>
@@ -2311,6 +2320,7 @@
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="22"/>
@@ -2318,6 +2328,7 @@
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="22"/>
@@ -2325,6 +2336,7 @@
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="22"/>
@@ -2332,6 +2344,7 @@
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="22"/>
@@ -2339,6 +2352,7 @@
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="22"/>
@@ -2346,6 +2360,7 @@
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
@@ -2383,46 +2398,46 @@
   <sheetData>
     <row r="1" ht="45.35" customHeight="1">
       <c r="A1" t="s" s="24">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s" s="25">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s" s="25">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s" s="25">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s" s="25">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s" s="26">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s" s="27">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s" s="27">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s" s="28">
         <v>18</v>
       </c>
       <c r="K1" t="s" s="21">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L1" t="s" s="21">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M1" t="s" s="21">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N1" t="s" s="21">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O1" s="22"/>
       <c r="P1" s="22"/>
@@ -2433,37 +2448,37 @@
       <c r="U1" s="22"/>
       <c r="V1" s="22"/>
       <c r="W1" t="s" s="29">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="24">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s" s="24">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s" s="24">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s" s="24">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s" s="24">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" t="b" s="30">
         <f t="shared" si="0" ref="F2:F3">FALSE</f>
         <v>0</v>
       </c>
       <c r="G2" t="s" s="26">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s" s="31">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I2" t="s" s="31">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J2" s="32"/>
       <c r="K2" s="22"/>
@@ -2471,10 +2486,10 @@
         <v>10</v>
       </c>
       <c r="M2" t="s" s="21">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N2" t="s" s="21">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
@@ -2485,7 +2500,7 @@
       <c r="U2" s="22"/>
       <c r="V2" s="22"/>
       <c r="W2" t="s" s="21">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="17" customHeight="1">
@@ -2493,40 +2508,40 @@
         <v>13</v>
       </c>
       <c r="B3" t="s" s="24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s" s="24">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="24">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s" s="24">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3" t="b" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G3" t="s" s="26">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" t="s" s="31">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J3" t="s" s="28">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K3" t="s" s="35">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" t="s" s="21">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N3" t="s" s="21">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
@@ -2824,40 +2839,40 @@
   <sheetData>
     <row r="1" ht="105.35" customHeight="1">
       <c r="A1" t="s" s="24">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s" s="24">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s" s="24">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s" s="25">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s" s="24">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s" s="25">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s" s="24">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s" s="24">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s" s="24">
         <v>18</v>
       </c>
       <c r="J1" t="s" s="24">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K1" t="s" s="24">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L1" t="s" s="25">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M1" s="39"/>
       <c r="N1" s="22"/>
@@ -2873,26 +2888,26 @@
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="24">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D2" t="b" s="30">
         <f t="shared" si="0" ref="D2:D14">TRUE</f>
         <v>1</v>
       </c>
       <c r="E2" t="s" s="24">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" s="40"/>
       <c r="H2" s="40"/>
       <c r="I2" t="s" s="24">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J2" s="30">
         <v>1</v>
@@ -2915,26 +2930,26 @@
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="24">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D3" t="b" s="30">
         <f t="shared" si="1" ref="D3:D20">FALSE</f>
         <v>0</v>
       </c>
       <c r="E3" t="s" s="24">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40"/>
       <c r="I3" t="s" s="24">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J3" s="30">
         <v>4</v>
@@ -2957,26 +2972,26 @@
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="24">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B4" s="40"/>
       <c r="C4" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D4" t="b" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E4" t="s" s="24">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G4" s="40"/>
       <c r="H4" s="40"/>
       <c r="I4" t="s" s="24">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J4" s="30">
         <v>16</v>
@@ -2999,11 +3014,11 @@
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="24">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B5" s="40"/>
       <c r="C5" t="s" s="24">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D5" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3011,14 +3026,14 @@
       </c>
       <c r="E5" s="40"/>
       <c r="F5" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" t="s" s="24">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I5" t="s" s="24">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J5" s="30">
         <v>17</v>
@@ -3041,11 +3056,11 @@
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="24">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B6" s="40"/>
       <c r="C6" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3053,12 +3068,12 @@
       </c>
       <c r="E6" s="40"/>
       <c r="F6" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
       <c r="I6" t="s" s="24">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J6" s="30">
         <v>27</v>
@@ -3081,13 +3096,13 @@
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" t="s" s="24">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s" s="24">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D7" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3095,12 +3110,12 @@
       </c>
       <c r="E7" s="40"/>
       <c r="F7" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
       <c r="I7" t="s" s="24">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J7" s="30">
         <v>46</v>
@@ -3123,11 +3138,11 @@
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" t="s" s="24">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D8" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3135,12 +3150,12 @@
       </c>
       <c r="E8" s="40"/>
       <c r="F8" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" t="s" s="24">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J8" s="30">
         <v>49</v>
@@ -3163,13 +3178,13 @@
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" t="s" s="24">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s" s="24">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D9" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3177,12 +3192,12 @@
       </c>
       <c r="E9" s="40"/>
       <c r="F9" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" t="s" s="24">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J9" s="30">
         <v>50</v>
@@ -3205,13 +3220,13 @@
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" t="s" s="24">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s" s="24">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3219,12 +3234,12 @@
       </c>
       <c r="E10" s="40"/>
       <c r="F10" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
       <c r="I10" t="s" s="24">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J10" s="30">
         <v>52</v>
@@ -3247,13 +3262,13 @@
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" t="s" s="24">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s" s="24">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D11" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3261,12 +3276,12 @@
       </c>
       <c r="E11" s="40"/>
       <c r="F11" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
       <c r="I11" t="s" s="24">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J11" s="30">
         <v>53</v>
@@ -3289,11 +3304,11 @@
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" t="s" s="24">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D12" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3301,14 +3316,14 @@
       </c>
       <c r="E12" s="40"/>
       <c r="F12" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s" s="24">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H12" s="40"/>
       <c r="I12" t="s" s="24">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12" s="30">
         <v>55</v>
@@ -3331,13 +3346,13 @@
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" t="s" s="24">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s" s="24">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3345,12 +3360,12 @@
       </c>
       <c r="E13" s="40"/>
       <c r="F13" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G13" s="40"/>
       <c r="H13" s="40"/>
       <c r="I13" t="s" s="24">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J13" s="30">
         <v>56</v>
@@ -3373,11 +3388,11 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="24">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D14" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3385,12 +3400,12 @@
       </c>
       <c r="E14" s="40"/>
       <c r="F14" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
       <c r="I14" t="s" s="24">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J14" s="30">
         <v>66</v>
@@ -3413,11 +3428,11 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="24">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3425,12 +3440,12 @@
       </c>
       <c r="E15" s="40"/>
       <c r="F15" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" t="s" s="24">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J15" s="30">
         <v>72</v>
@@ -3453,11 +3468,11 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="24">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3465,12 +3480,12 @@
       </c>
       <c r="E16" s="40"/>
       <c r="F16" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
       <c r="I16" t="s" s="24">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J16" s="30">
         <v>77</v>
@@ -3493,11 +3508,11 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="24">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3505,12 +3520,12 @@
       </c>
       <c r="E17" s="40"/>
       <c r="F17" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G17" s="40"/>
       <c r="H17" s="40"/>
       <c r="I17" t="s" s="24">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J17" s="30">
         <v>82</v>
@@ -3533,11 +3548,11 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="24">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3545,12 +3560,12 @@
       </c>
       <c r="E18" s="40"/>
       <c r="F18" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G18" s="40"/>
       <c r="H18" s="40"/>
       <c r="I18" t="s" s="24">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J18" s="30">
         <v>87</v>
@@ -3573,13 +3588,13 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="24">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s" s="24">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3587,12 +3602,12 @@
       </c>
       <c r="E19" s="40"/>
       <c r="F19" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
       <c r="I19" t="s" s="24">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J19" s="30">
         <v>92</v>
@@ -3615,11 +3630,11 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="24">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3627,12 +3642,12 @@
       </c>
       <c r="E20" s="40"/>
       <c r="F20" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" t="s" s="24">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J20" s="30">
         <v>93</v>
@@ -3678,13 +3693,13 @@
   <sheetData>
     <row r="1" ht="17.9" customHeight="1">
       <c r="A1" t="s" s="29">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s" s="29">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C1" t="s" s="29">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D1" t="s" s="29">
         <v>18</v>
@@ -3693,26 +3708,26 @@
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="21">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s" s="21">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s" s="21">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="21">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s" s="21">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s" s="21">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -3798,49 +3813,49 @@
   <sheetData>
     <row r="1" ht="105.35" customHeight="1">
       <c r="A1" t="s" s="24">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s" s="24">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s" s="24">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s" s="25">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s" s="24">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s" s="25">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s" s="24">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s" s="24">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s" s="24">
         <v>18</v>
       </c>
       <c r="J1" t="s" s="24">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K1" t="s" s="24">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L1" t="s" s="25">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="24">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D2" t="b" s="30">
         <f t="shared" si="0" ref="D2:D20">TRUE</f>
@@ -3848,12 +3863,12 @@
       </c>
       <c r="E2" s="40"/>
       <c r="F2" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" s="40"/>
       <c r="H2" s="40"/>
       <c r="I2" t="s" s="24">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J2" s="40"/>
       <c r="K2" s="40"/>
@@ -3861,11 +3876,11 @@
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="24">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" t="s" s="24">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3873,12 +3888,12 @@
       </c>
       <c r="E3" s="40"/>
       <c r="F3" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40"/>
       <c r="I3" t="s" s="24">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J3" s="40"/>
       <c r="K3" s="40"/>
@@ -3886,11 +3901,11 @@
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="24">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B4" s="40"/>
       <c r="C4" t="s" s="24">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D4" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3898,12 +3913,12 @@
       </c>
       <c r="E4" s="40"/>
       <c r="F4" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G4" s="40"/>
       <c r="H4" s="40"/>
       <c r="I4" t="s" s="24">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
@@ -3911,11 +3926,11 @@
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="24">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B5" s="40"/>
       <c r="C5" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D5" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3923,12 +3938,12 @@
       </c>
       <c r="E5" s="40"/>
       <c r="F5" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" s="40"/>
       <c r="I5" t="s" s="24">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J5" s="40"/>
       <c r="K5" s="40"/>
@@ -3936,11 +3951,11 @@
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="24">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B6" s="40"/>
       <c r="C6" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3948,12 +3963,12 @@
       </c>
       <c r="E6" s="40"/>
       <c r="F6" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
       <c r="I6" t="s" s="24">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J6" s="40"/>
       <c r="K6" s="40"/>
@@ -3961,11 +3976,11 @@
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" t="s" s="24">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B7" s="40"/>
       <c r="C7" t="s" s="24">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D7" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3973,12 +3988,12 @@
       </c>
       <c r="E7" s="40"/>
       <c r="F7" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
       <c r="I7" t="s" s="24">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J7" s="40"/>
       <c r="K7" s="40"/>
@@ -3986,11 +4001,11 @@
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" t="s" s="24">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" t="s" s="24">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D8" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3998,12 +4013,12 @@
       </c>
       <c r="E8" s="40"/>
       <c r="F8" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" t="s" s="24">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J8" s="40"/>
       <c r="K8" s="40"/>
@@ -4011,26 +4026,26 @@
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" t="s" s="24">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B9" s="40"/>
       <c r="C9" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D9" t="b" s="30">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E9" t="s" s="24">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" t="s" s="24">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J9" s="40"/>
       <c r="K9" s="40"/>
@@ -4038,26 +4053,26 @@
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" t="s" s="24">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B10" s="40"/>
       <c r="C10" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" t="b" s="30">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E10" t="s" s="24">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
       <c r="I10" t="s" s="24">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J10" s="40"/>
       <c r="K10" s="40"/>
@@ -4065,11 +4080,11 @@
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" t="s" s="24">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D11" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4077,12 +4092,12 @@
       </c>
       <c r="E11" s="40"/>
       <c r="F11" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
       <c r="I11" t="s" s="24">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J11" s="40"/>
       <c r="K11" s="40"/>
@@ -4090,11 +4105,11 @@
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" t="s" s="24">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" t="s" s="24">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D12" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4102,12 +4117,12 @@
       </c>
       <c r="E12" s="40"/>
       <c r="F12" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G12" s="40"/>
       <c r="H12" s="40"/>
       <c r="I12" t="s" s="24">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12" s="40"/>
       <c r="K12" s="40"/>
@@ -4115,11 +4130,11 @@
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" t="s" s="24">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4127,12 +4142,12 @@
       </c>
       <c r="E13" s="40"/>
       <c r="F13" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G13" s="40"/>
       <c r="H13" s="40"/>
       <c r="I13" t="s" s="24">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J13" s="40"/>
       <c r="K13" s="40"/>
@@ -4140,11 +4155,11 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="24">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D14" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4152,12 +4167,12 @@
       </c>
       <c r="E14" s="40"/>
       <c r="F14" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
       <c r="I14" t="s" s="24">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J14" s="40"/>
       <c r="K14" s="40"/>
@@ -4165,11 +4180,11 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="24">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4177,12 +4192,12 @@
       </c>
       <c r="E15" s="40"/>
       <c r="F15" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" t="s" s="24">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
@@ -4190,11 +4205,11 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="24">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4202,12 +4217,12 @@
       </c>
       <c r="E16" s="40"/>
       <c r="F16" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
       <c r="I16" t="s" s="24">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J16" s="40"/>
       <c r="K16" s="40"/>
@@ -4215,11 +4230,11 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="24">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" t="s" s="24">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D17" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4227,12 +4242,12 @@
       </c>
       <c r="E17" s="40"/>
       <c r="F17" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G17" s="40"/>
       <c r="H17" s="40"/>
       <c r="I17" t="s" s="24">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
@@ -4240,11 +4255,11 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="24">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4252,12 +4267,12 @@
       </c>
       <c r="E18" s="40"/>
       <c r="F18" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G18" s="40"/>
       <c r="H18" s="40"/>
       <c r="I18" t="s" s="24">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J18" s="40"/>
       <c r="K18" s="40"/>
@@ -4265,11 +4280,11 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="24">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4277,12 +4292,12 @@
       </c>
       <c r="E19" s="40"/>
       <c r="F19" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
       <c r="I19" t="s" s="24">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J19" s="40"/>
       <c r="K19" s="40"/>
@@ -4290,11 +4305,11 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="24">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" t="s" s="24">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4302,12 +4317,12 @@
       </c>
       <c r="E20" s="40"/>
       <c r="F20" t="s" s="24">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" t="s" s="24">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J20" s="40"/>
       <c r="K20" s="40"/>

</xml_diff>

<commit_message>
to allow no partitoning column with BQ
</commit_message>
<xml_diff>
--- a/src/test/resources/sample/SomeDomainTemplate.xlsx
+++ b/src/test/resources/sample/SomeDomainTemplate.xlsx
@@ -11,12 +11,13 @@
     <sheet name="SCHEMA1" sheetId="4" r:id="rId7"/>
     <sheet name="_policies" sheetId="5" r:id="rId8"/>
     <sheet name="SCHEMA2" sheetId="6" r:id="rId9"/>
+    <sheet name="SCHEMA3" sheetId="7" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="152">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -235,6 +236,15 @@
   </si>
   <si>
     <t>RENAME_ATTRIBUTE_8, RENAME_ATTRIBUTE_9</t>
+  </si>
+  <si>
+    <t>SCHEMA3</t>
+  </si>
+  <si>
+    <t>SomeFile3_*.csv</t>
+  </si>
+  <si>
+    <t>BQ</t>
   </si>
   <si>
     <t>NomTechnique</t>
@@ -814,7 +824,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -936,6 +946,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2468,7 +2481,7 @@
         <v>43</v>
       </c>
       <c r="F2" t="b" s="30">
-        <f t="shared" si="0" ref="F2:F3">FALSE</f>
+        <f t="shared" si="0" ref="F2:F4">FALSE</f>
         <v>0</v>
       </c>
       <c r="G2" t="s" s="26">
@@ -2554,20 +2567,37 @@
       <c r="W3" s="22"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="A4" t="s" s="24">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s" s="24">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s" s="24">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s" s="24">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s" s="24">
+        <v>52</v>
+      </c>
+      <c r="F4" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" t="s" s="26">
+        <v>53</v>
+      </c>
+      <c r="H4" s="34"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="35"/>
       <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
+      <c r="M4" s="21"/>
+      <c r="N4" t="s" s="21">
+        <v>60</v>
+      </c>
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
       <c r="Q4" s="22"/>
@@ -2579,15 +2609,15 @@
       <c r="W4" s="22"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
@@ -2839,40 +2869,40 @@
   <sheetData>
     <row r="1" ht="105.35" customHeight="1">
       <c r="A1" t="s" s="24">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s" s="24">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s" s="24">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s" s="25">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s" s="24">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s" s="25">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s" s="24">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s" s="24">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s" s="24">
         <v>18</v>
       </c>
       <c r="J1" t="s" s="24">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K1" t="s" s="24">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L1" t="s" s="25">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="M1" s="39"/>
       <c r="N1" s="22"/>
@@ -2892,22 +2922,22 @@
       </c>
       <c r="B2" s="40"/>
       <c r="C2" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D2" t="b" s="30">
         <f t="shared" si="0" ref="D2:D14">TRUE</f>
         <v>1</v>
       </c>
       <c r="E2" t="s" s="24">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G2" s="40"/>
       <c r="H2" s="40"/>
       <c r="I2" t="s" s="24">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J2" s="30">
         <v>1</v>
@@ -2930,26 +2960,26 @@
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="24">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D3" t="b" s="30">
         <f t="shared" si="1" ref="D3:D20">FALSE</f>
         <v>0</v>
       </c>
       <c r="E3" t="s" s="24">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40"/>
       <c r="I3" t="s" s="24">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J3" s="30">
         <v>4</v>
@@ -2972,26 +3002,26 @@
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="24">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B4" s="40"/>
       <c r="C4" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D4" t="b" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E4" t="s" s="24">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G4" s="40"/>
       <c r="H4" s="40"/>
       <c r="I4" t="s" s="24">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J4" s="30">
         <v>16</v>
@@ -3014,11 +3044,11 @@
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="24">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B5" s="40"/>
       <c r="C5" t="s" s="24">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D5" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3026,14 +3056,14 @@
       </c>
       <c r="E5" s="40"/>
       <c r="F5" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" t="s" s="24">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I5" t="s" s="24">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J5" s="30">
         <v>17</v>
@@ -3056,11 +3086,11 @@
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="24">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B6" s="40"/>
       <c r="C6" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D6" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3068,12 +3098,12 @@
       </c>
       <c r="E6" s="40"/>
       <c r="F6" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
       <c r="I6" t="s" s="24">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J6" s="30">
         <v>27</v>
@@ -3096,13 +3126,13 @@
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" t="s" s="24">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s" s="24">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D7" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3110,12 +3140,12 @@
       </c>
       <c r="E7" s="40"/>
       <c r="F7" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
       <c r="I7" t="s" s="24">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J7" s="30">
         <v>46</v>
@@ -3138,11 +3168,11 @@
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" t="s" s="24">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D8" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3150,12 +3180,12 @@
       </c>
       <c r="E8" s="40"/>
       <c r="F8" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" t="s" s="24">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J8" s="30">
         <v>49</v>
@@ -3178,13 +3208,13 @@
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" t="s" s="24">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s" s="24">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D9" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3192,12 +3222,12 @@
       </c>
       <c r="E9" s="40"/>
       <c r="F9" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" t="s" s="24">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J9" s="30">
         <v>50</v>
@@ -3220,13 +3250,13 @@
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" t="s" s="24">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s" s="24">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D10" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3234,12 +3264,12 @@
       </c>
       <c r="E10" s="40"/>
       <c r="F10" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
       <c r="I10" t="s" s="24">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J10" s="30">
         <v>52</v>
@@ -3262,13 +3292,13 @@
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" t="s" s="24">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s" s="24">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D11" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3276,12 +3306,12 @@
       </c>
       <c r="E11" s="40"/>
       <c r="F11" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
       <c r="I11" t="s" s="24">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J11" s="30">
         <v>53</v>
@@ -3304,11 +3334,11 @@
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" t="s" s="24">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D12" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3316,14 +3346,14 @@
       </c>
       <c r="E12" s="40"/>
       <c r="F12" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s" s="24">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H12" s="40"/>
       <c r="I12" t="s" s="24">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J12" s="30">
         <v>55</v>
@@ -3346,13 +3376,13 @@
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" t="s" s="24">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s" s="24">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D13" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3360,12 +3390,12 @@
       </c>
       <c r="E13" s="40"/>
       <c r="F13" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G13" s="40"/>
       <c r="H13" s="40"/>
       <c r="I13" t="s" s="24">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="J13" s="30">
         <v>56</v>
@@ -3388,11 +3418,11 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="24">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D14" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3400,12 +3430,12 @@
       </c>
       <c r="E14" s="40"/>
       <c r="F14" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
       <c r="I14" t="s" s="24">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J14" s="30">
         <v>66</v>
@@ -3428,11 +3458,11 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="24">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D15" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3440,12 +3470,12 @@
       </c>
       <c r="E15" s="40"/>
       <c r="F15" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" t="s" s="24">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J15" s="30">
         <v>72</v>
@@ -3468,11 +3498,11 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="24">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D16" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3480,12 +3510,12 @@
       </c>
       <c r="E16" s="40"/>
       <c r="F16" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
       <c r="I16" t="s" s="24">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J16" s="30">
         <v>77</v>
@@ -3508,11 +3538,11 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="24">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D17" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3520,12 +3550,12 @@
       </c>
       <c r="E17" s="40"/>
       <c r="F17" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G17" s="40"/>
       <c r="H17" s="40"/>
       <c r="I17" t="s" s="24">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="J17" s="30">
         <v>82</v>
@@ -3548,11 +3578,11 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="24">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D18" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3560,12 +3590,12 @@
       </c>
       <c r="E18" s="40"/>
       <c r="F18" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G18" s="40"/>
       <c r="H18" s="40"/>
       <c r="I18" t="s" s="24">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="J18" s="30">
         <v>87</v>
@@ -3588,13 +3618,13 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="24">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s" s="24">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D19" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3602,12 +3632,12 @@
       </c>
       <c r="E19" s="40"/>
       <c r="F19" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
       <c r="I19" t="s" s="24">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="J19" s="30">
         <v>92</v>
@@ -3634,7 +3664,7 @@
       </c>
       <c r="B20" s="40"/>
       <c r="C20" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D20" t="b" s="30">
         <f t="shared" si="1"/>
@@ -3642,12 +3672,12 @@
       </c>
       <c r="E20" s="40"/>
       <c r="F20" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" t="s" s="24">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J20" s="30">
         <v>93</v>
@@ -3685,21 +3715,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16667" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="9.17188" style="41" customWidth="1"/>
-    <col min="3" max="3" width="19.1719" style="41" customWidth="1"/>
+    <col min="1" max="1" width="9.17188" style="41" customWidth="1"/>
+    <col min="2" max="2" width="14.6484" style="41" customWidth="1"/>
+    <col min="3" max="3" width="28.1641" style="41" customWidth="1"/>
     <col min="4" max="5" width="9.17188" style="41" customWidth="1"/>
     <col min="6" max="16384" width="9.17188" style="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.9" customHeight="1">
       <c r="A1" t="s" s="29">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s" s="29">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C1" t="s" s="29">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s" s="29">
         <v>18</v>
@@ -3708,26 +3739,26 @@
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="21">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s" s="21">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s" s="21">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="21">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s" s="21">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s" s="21">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -3813,49 +3844,49 @@
   <sheetData>
     <row r="1" ht="105.35" customHeight="1">
       <c r="A1" t="s" s="24">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s" s="24">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s" s="24">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s" s="25">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s" s="24">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F1" t="s" s="25">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s" s="24">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s" s="24">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s" s="24">
         <v>18</v>
       </c>
       <c r="J1" t="s" s="24">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K1" t="s" s="24">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L1" t="s" s="25">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="24">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D2" t="b" s="30">
         <f t="shared" si="0" ref="D2:D20">TRUE</f>
@@ -3863,12 +3894,12 @@
       </c>
       <c r="E2" s="40"/>
       <c r="F2" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G2" s="40"/>
       <c r="H2" s="40"/>
       <c r="I2" t="s" s="24">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J2" s="40"/>
       <c r="K2" s="40"/>
@@ -3876,11 +3907,11 @@
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="24">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" t="s" s="24">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D3" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3888,12 +3919,12 @@
       </c>
       <c r="E3" s="40"/>
       <c r="F3" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40"/>
       <c r="I3" t="s" s="24">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J3" s="40"/>
       <c r="K3" s="40"/>
@@ -3901,11 +3932,11 @@
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="24">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B4" s="40"/>
       <c r="C4" t="s" s="24">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D4" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3913,12 +3944,12 @@
       </c>
       <c r="E4" s="40"/>
       <c r="F4" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G4" s="40"/>
       <c r="H4" s="40"/>
       <c r="I4" t="s" s="24">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
@@ -3926,11 +3957,11 @@
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="24">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B5" s="40"/>
       <c r="C5" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D5" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3938,12 +3969,12 @@
       </c>
       <c r="E5" s="40"/>
       <c r="F5" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" s="40"/>
       <c r="I5" t="s" s="24">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J5" s="40"/>
       <c r="K5" s="40"/>
@@ -3951,11 +3982,11 @@
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="24">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B6" s="40"/>
       <c r="C6" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D6" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3963,12 +3994,12 @@
       </c>
       <c r="E6" s="40"/>
       <c r="F6" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
       <c r="I6" t="s" s="24">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J6" s="40"/>
       <c r="K6" s="40"/>
@@ -3976,11 +4007,11 @@
     </row>
     <row r="7" ht="15.35" customHeight="1">
       <c r="A7" t="s" s="24">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B7" s="40"/>
       <c r="C7" t="s" s="24">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D7" t="b" s="30">
         <f t="shared" si="0"/>
@@ -3988,12 +4019,12 @@
       </c>
       <c r="E7" s="40"/>
       <c r="F7" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
       <c r="I7" t="s" s="24">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J7" s="40"/>
       <c r="K7" s="40"/>
@@ -4001,11 +4032,11 @@
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" t="s" s="24">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" t="s" s="24">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D8" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4013,12 +4044,12 @@
       </c>
       <c r="E8" s="40"/>
       <c r="F8" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
       <c r="I8" t="s" s="24">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J8" s="40"/>
       <c r="K8" s="40"/>
@@ -4026,26 +4057,26 @@
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" t="s" s="24">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B9" s="40"/>
       <c r="C9" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D9" t="b" s="30">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E9" t="s" s="24">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F9" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
       <c r="I9" t="s" s="24">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="J9" s="40"/>
       <c r="K9" s="40"/>
@@ -4053,26 +4084,26 @@
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" t="s" s="24">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B10" s="40"/>
       <c r="C10" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D10" t="b" s="30">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E10" t="s" s="24">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
       <c r="I10" t="s" s="24">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J10" s="40"/>
       <c r="K10" s="40"/>
@@ -4080,11 +4111,11 @@
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" t="s" s="24">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D11" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4092,12 +4123,12 @@
       </c>
       <c r="E11" s="40"/>
       <c r="F11" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
       <c r="I11" t="s" s="24">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J11" s="40"/>
       <c r="K11" s="40"/>
@@ -4105,11 +4136,11 @@
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" t="s" s="24">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" t="s" s="24">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D12" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4117,12 +4148,12 @@
       </c>
       <c r="E12" s="40"/>
       <c r="F12" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G12" s="40"/>
       <c r="H12" s="40"/>
       <c r="I12" t="s" s="24">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J12" s="40"/>
       <c r="K12" s="40"/>
@@ -4130,11 +4161,11 @@
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" t="s" s="24">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D13" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4142,12 +4173,12 @@
       </c>
       <c r="E13" s="40"/>
       <c r="F13" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G13" s="40"/>
       <c r="H13" s="40"/>
       <c r="I13" t="s" s="24">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="J13" s="40"/>
       <c r="K13" s="40"/>
@@ -4155,11 +4186,11 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="24">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D14" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4167,12 +4198,12 @@
       </c>
       <c r="E14" s="40"/>
       <c r="F14" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
       <c r="I14" t="s" s="24">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J14" s="40"/>
       <c r="K14" s="40"/>
@@ -4180,11 +4211,11 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="24">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B15" s="40"/>
       <c r="C15" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D15" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4192,12 +4223,12 @@
       </c>
       <c r="E15" s="40"/>
       <c r="F15" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" t="s" s="24">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
@@ -4205,11 +4236,11 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="24">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D16" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4217,12 +4248,12 @@
       </c>
       <c r="E16" s="40"/>
       <c r="F16" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G16" s="40"/>
       <c r="H16" s="40"/>
       <c r="I16" t="s" s="24">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J16" s="40"/>
       <c r="K16" s="40"/>
@@ -4230,11 +4261,11 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="24">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B17" s="40"/>
       <c r="C17" t="s" s="24">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D17" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4242,12 +4273,12 @@
       </c>
       <c r="E17" s="40"/>
       <c r="F17" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G17" s="40"/>
       <c r="H17" s="40"/>
       <c r="I17" t="s" s="24">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
@@ -4255,11 +4286,11 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="24">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D18" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4267,12 +4298,12 @@
       </c>
       <c r="E18" s="40"/>
       <c r="F18" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G18" s="40"/>
       <c r="H18" s="40"/>
       <c r="I18" t="s" s="24">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="J18" s="40"/>
       <c r="K18" s="40"/>
@@ -4280,11 +4311,11 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="24">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D19" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4292,12 +4323,12 @@
       </c>
       <c r="E19" s="40"/>
       <c r="F19" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
       <c r="I19" t="s" s="24">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="J19" s="40"/>
       <c r="K19" s="40"/>
@@ -4305,11 +4336,11 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="24">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B20" s="40"/>
       <c r="C20" t="s" s="24">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D20" t="b" s="30">
         <f t="shared" si="0"/>
@@ -4317,12 +4348,559 @@
       </c>
       <c r="E20" s="40"/>
       <c r="F20" t="s" s="24">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" t="s" s="24">
+        <v>120</v>
+      </c>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="23.5" style="43" customWidth="1"/>
+    <col min="2" max="2" width="15.1719" style="43" customWidth="1"/>
+    <col min="3" max="3" width="16" style="43" customWidth="1"/>
+    <col min="4" max="4" width="10.6719" style="43" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="43" customWidth="1"/>
+    <col min="6" max="6" width="23" style="43" customWidth="1"/>
+    <col min="7" max="7" width="16.3516" style="43" customWidth="1"/>
+    <col min="8" max="8" width="16.1719" style="43" customWidth="1"/>
+    <col min="9" max="9" width="30.3516" style="43" customWidth="1"/>
+    <col min="10" max="12" width="10.8516" style="43" customWidth="1"/>
+    <col min="13" max="16384" width="10.8516" style="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="105.35" customHeight="1">
+      <c r="A1" t="s" s="24">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s" s="24">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s" s="25">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s" s="24">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s" s="25">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s" s="24">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s" s="24">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s" s="24">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s" s="24">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s" s="24">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s" s="25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" ht="15.35" customHeight="1">
+      <c r="A2" t="s" s="24">
+        <v>130</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D2" t="b" s="30">
+        <f t="shared" si="0" ref="D2:D20">TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="40"/>
+      <c r="F2" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" t="s" s="24">
+        <v>75</v>
+      </c>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+    </row>
+    <row r="3" ht="15.35" customHeight="1">
+      <c r="A3" t="s" s="24">
+        <v>131</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" t="s" s="24">
+        <v>83</v>
+      </c>
+      <c r="D3" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="F3" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" t="s" s="24">
+        <v>78</v>
+      </c>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+    </row>
+    <row r="4" ht="15.35" customHeight="1">
+      <c r="A4" t="s" s="24">
+        <v>132</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" t="s" s="24">
+        <v>133</v>
+      </c>
+      <c r="D4" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" t="s" s="24">
+        <v>81</v>
+      </c>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+    </row>
+    <row r="5" ht="15.35" customHeight="1">
+      <c r="A5" t="s" s="24">
+        <v>134</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D5" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" t="s" s="24">
+        <v>85</v>
+      </c>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+    </row>
+    <row r="6" ht="15.35" customHeight="1">
+      <c r="A6" t="s" s="24">
+        <v>135</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D6" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="40"/>
+      <c r="F6" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" t="s" s="24">
+        <v>87</v>
+      </c>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1">
+      <c r="A7" t="s" s="24">
+        <v>136</v>
+      </c>
+      <c r="B7" s="40"/>
+      <c r="C7" t="s" s="24">
+        <v>137</v>
+      </c>
+      <c r="D7" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" t="s" s="24">
+        <v>90</v>
+      </c>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" t="s" s="24">
+        <v>138</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" t="s" s="24">
+        <v>137</v>
+      </c>
+      <c r="D8" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" t="s" s="24">
+        <v>92</v>
+      </c>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" t="s" s="24">
+        <v>139</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D9" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" t="s" s="24">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" t="s" s="24">
+        <v>95</v>
+      </c>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" t="s" s="24">
+        <v>140</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D10" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" t="s" s="24">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" t="s" s="24">
+        <v>98</v>
+      </c>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+    </row>
+    <row r="11" ht="15.35" customHeight="1">
+      <c r="A11" t="s" s="24">
+        <v>141</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D11" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" t="s" s="24">
+        <v>101</v>
+      </c>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+    </row>
+    <row r="12" ht="15.35" customHeight="1">
+      <c r="A12" t="s" s="24">
+        <v>142</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" t="s" s="24">
+        <v>143</v>
+      </c>
+      <c r="D12" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="40"/>
+      <c r="F12" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" t="s" s="24">
+        <v>104</v>
+      </c>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+    </row>
+    <row r="13" ht="15.35" customHeight="1">
+      <c r="A13" t="s" s="24">
+        <v>144</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D13" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" t="s" s="24">
+        <v>107</v>
+      </c>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+    </row>
+    <row r="14" ht="15.35" customHeight="1">
+      <c r="A14" t="s" s="24">
+        <v>145</v>
+      </c>
+      <c r="B14" s="40"/>
+      <c r="C14" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D14" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" t="s" s="24">
+        <v>109</v>
+      </c>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+    </row>
+    <row r="15" ht="15.35" customHeight="1">
+      <c r="A15" t="s" s="24">
+        <v>146</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D15" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" t="s" s="24">
+        <v>111</v>
+      </c>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+    </row>
+    <row r="16" ht="15.35" customHeight="1">
+      <c r="A16" t="s" s="24">
+        <v>147</v>
+      </c>
+      <c r="B16" s="40"/>
+      <c r="C16" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D16" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" t="s" s="24">
+        <v>113</v>
+      </c>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+    </row>
+    <row r="17" ht="15.35" customHeight="1">
+      <c r="A17" t="s" s="24">
+        <v>148</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" t="s" s="24">
+        <v>83</v>
+      </c>
+      <c r="D17" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" t="s" s="24">
+        <v>115</v>
+      </c>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+    </row>
+    <row r="18" ht="15.35" customHeight="1">
+      <c r="A18" t="s" s="24">
+        <v>149</v>
+      </c>
+      <c r="B18" s="40"/>
+      <c r="C18" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D18" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="40"/>
+      <c r="F18" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" t="s" s="24">
         <v>117</v>
+      </c>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+    </row>
+    <row r="19" ht="15.35" customHeight="1">
+      <c r="A19" t="s" s="24">
+        <v>150</v>
+      </c>
+      <c r="B19" s="40"/>
+      <c r="C19" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D19" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" t="s" s="24">
+        <v>119</v>
+      </c>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+    </row>
+    <row r="20" ht="15.35" customHeight="1">
+      <c r="A20" t="s" s="24">
+        <v>151</v>
+      </c>
+      <c r="B20" s="40"/>
+      <c r="C20" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D20" t="b" s="30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" t="s" s="24">
+        <v>74</v>
+      </c>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" t="s" s="24">
+        <v>120</v>
       </c>
       <c r="J20" s="40"/>
       <c r="K20" s="40"/>

</xml_diff>